<commit_message>
implement dh price into data prep
the dh price is now taken from the price cap xlsx sheet.
</commit_message>
<xml_diff>
--- a/spine_projects/01_input_data/01_input_raw/energy_prices/district_heating_price_cap.xlsx
+++ b/spine_projects/01_input_data/01_input_raw/energy_prices/district_heating_price_cap.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jfg.eco\Documents\GitHub\Nord_H2ub\spine_projects\01_input_data\01_input_raw\energy_prices\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0159D30D-5DE0-43D1-BE79-4BFCEE0C1046}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F00FFD3-894A-456A-96BF-9C096690F073}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{BDF52CB5-8AF7-4070-9BAF-21BBD77363FF}"/>
   </bookViews>
   <sheets>
     <sheet name="Price_Cap_Calculation" sheetId="1" r:id="rId1"/>
-    <sheet name="Sources" sheetId="2" r:id="rId2"/>
+    <sheet name="Data" sheetId="3" r:id="rId2"/>
+    <sheet name="Sources" sheetId="2" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -59,7 +60,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="20">
   <si>
     <t>Law</t>
   </si>
@@ -110,13 +111,22 @@
   </si>
   <si>
     <t>Price cap</t>
+  </si>
+  <si>
+    <t>2021</t>
+  </si>
+  <si>
+    <t>2020</t>
+  </si>
+  <si>
+    <t>2019</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -124,16 +134,36 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor theme="4"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor theme="4" tint="0.79998168889431442"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -141,17 +171,127 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </top>
+      <bottom style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </right>
+      <top style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </top>
+      <bottom style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="4">
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="4" tint="0.79998168889431442"/>
+          <bgColor theme="4" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </top>
+        <bottom style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="4" tint="0.79998168889431442"/>
+          <bgColor theme="4" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </top>
+        <bottom style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <right style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </right>
+      </border>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -165,8 +305,25 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{0D0EDFBA-F446-4D1D-A165-86C53C97EEF2}" name="Table1" displayName="Table1" ref="G1:H2" totalsRowShown="0">
-  <autoFilter ref="G1:H2" xr:uid="{0D0EDFBA-F446-4D1D-A165-86C53C97EEF2}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{8F68E1AD-1E8B-4ACE-A9DE-2514707D9B42}" name="Table4" displayName="Table4" ref="A1:F4" totalsRowShown="0">
+  <autoFilter ref="A1:F4" xr:uid="{8F68E1AD-1E8B-4ACE-A9DE-2514707D9B42}"/>
+  <tableColumns count="6">
+    <tableColumn id="1" xr3:uid="{A6FEAB50-FA63-446B-B963-FFE2083525E3}" name="Price cap"/>
+    <tableColumn id="2" xr3:uid="{E77E28C3-6031-4C08-B54D-35A5A0CCC2F3}" name="2019"/>
+    <tableColumn id="3" xr3:uid="{9BF1D066-C7E0-4A13-8E0A-07795D412DD6}" name="2020"/>
+    <tableColumn id="4" xr3:uid="{94EEE701-C19A-4405-B469-9A9B9CFF43D5}" name="2021" dataDxfId="0">
+      <calculatedColumnFormula array="1">Table2[2019]</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="5" xr3:uid="{8EC6DBC7-5CD1-4CC1-B48E-052446EA7F03}" name="2022"/>
+    <tableColumn id="6" xr3:uid="{CE5F0BFC-0E32-4299-85B7-B0940B445FB9}" name="2023"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{0D0EDFBA-F446-4D1D-A165-86C53C97EEF2}" name="Table1" displayName="Table1" ref="A1:B2" totalsRowShown="0">
+  <autoFilter ref="A1:B2" xr:uid="{0D0EDFBA-F446-4D1D-A165-86C53C97EEF2}"/>
   <tableColumns count="2">
     <tableColumn id="1" xr3:uid="{99663915-0614-4914-A715-2C3741FC1ACC}" name="Exchange Rate"/>
     <tableColumn id="2" xr3:uid="{654AC930-73A7-43A5-96FC-7EBC23349791}" name="kr./Euro"/>
@@ -175,9 +332,9 @@
 </table>
 </file>
 
-<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{4E3300EA-E05E-4C87-BDBD-255FD5143D31}" name="Table3" displayName="Table3" ref="J1:K2" totalsRowShown="0">
-  <autoFilter ref="J1:K2" xr:uid="{4E3300EA-E05E-4C87-BDBD-255FD5143D31}"/>
+<file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{4E3300EA-E05E-4C87-BDBD-255FD5143D31}" name="Table3" displayName="Table3" ref="D1:E2" totalsRowShown="0">
+  <autoFilter ref="D1:E2" xr:uid="{4E3300EA-E05E-4C87-BDBD-255FD5143D31}"/>
   <tableColumns count="2">
     <tableColumn id="1" xr3:uid="{DDB901A1-8B1F-4758-9CE3-50B5E8E456D3}" name="Energy data"/>
     <tableColumn id="2" xr3:uid="{69F6EA6A-30F2-4D44-956C-0E4082DA3B9A}" name="Column1"/>
@@ -186,13 +343,16 @@
 </table>
 </file>
 
-<file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{8F68E1AD-1E8B-4ACE-A9DE-2514707D9B42}" name="Table4" displayName="Table4" ref="A1:C4" totalsRowShown="0">
-  <autoFilter ref="A1:C4" xr:uid="{8F68E1AD-1E8B-4ACE-A9DE-2514707D9B42}"/>
-  <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{A6FEAB50-FA63-446B-B963-FFE2083525E3}" name="Price cap"/>
-    <tableColumn id="2" xr3:uid="{E77E28C3-6031-4C08-B54D-35A5A0CCC2F3}" name="2022"/>
-    <tableColumn id="3" xr3:uid="{9BF1D066-C7E0-4A13-8E0A-07795D412DD6}" name="2023"/>
+<file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{7BF6279C-0A47-4882-8A47-FBB883A7F586}" name="Table2" displayName="Table2" ref="A5:F6" totalsRowShown="0" tableBorderDxfId="3">
+  <autoFilter ref="A5:F6" xr:uid="{7BF6279C-0A47-4882-8A47-FBB883A7F586}"/>
+  <tableColumns count="6">
+    <tableColumn id="1" xr3:uid="{D3E85E44-117A-4A3D-B167-80884115B936}" name="Price cap"/>
+    <tableColumn id="2" xr3:uid="{9FB8A1A3-5B94-42D9-8374-F609ECDC4806}" name="2019"/>
+    <tableColumn id="3" xr3:uid="{BC877BDF-034D-4BAE-8945-44CE9F9FA3BF}" name="2020"/>
+    <tableColumn id="4" xr3:uid="{C3208B9F-5220-4737-97F7-04B4B458599B}" name="2021"/>
+    <tableColumn id="5" xr3:uid="{717424EF-4D50-42EC-ABE0-707DA0FB5BFE}" name="2022" dataDxfId="2"/>
+    <tableColumn id="6" xr3:uid="{7B8608B1-3E6A-44D6-B820-4DE5304A1F9D}" name="2023" dataDxfId="1"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -515,10 +675,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{38179E1F-D8DC-462A-A2B6-DE363F6626F8}">
-  <dimension ref="A1:K4"/>
+  <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="I11" sqref="I11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -530,53 +690,52 @@
     <col min="11" max="11" width="10.453125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>16</v>
       </c>
       <c r="B1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="C1" t="s">
+      <c r="F1" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="G1" t="s">
-        <v>6</v>
-      </c>
-      <c r="H1" t="s">
-        <v>7</v>
-      </c>
-      <c r="J1" t="s">
-        <v>10</v>
-      </c>
-      <c r="K1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.35">
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>5</v>
       </c>
-      <c r="B2">
+      <c r="B2" cm="1">
+        <f t="array" ref="B2">Table2[2019]</f>
         <v>77</v>
       </c>
-      <c r="C2">
+      <c r="C2" cm="1">
+        <f t="array" ref="C2">Table2[2020]</f>
+        <v>77</v>
+      </c>
+      <c r="D2" cm="1">
+        <f t="array" ref="D2">Table2[2021]</f>
+        <v>77</v>
+      </c>
+      <c r="E2" cm="1">
+        <f t="array" ref="E2">Table2[2022]</f>
+        <v>77</v>
+      </c>
+      <c r="F2" cm="1">
+        <f t="array" ref="F2">Table2[2023]</f>
         <v>93</v>
       </c>
-      <c r="G2" t="s">
-        <v>8</v>
-      </c>
-      <c r="H2">
-        <v>7.46</v>
-      </c>
-      <c r="J2" t="s">
-        <v>11</v>
-      </c>
-      <c r="K2">
-        <v>3.6</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.35">
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>9</v>
       </c>
@@ -586,10 +745,22 @@
       </c>
       <c r="C3" cm="1">
         <f t="array" ref="C3">C2/Table1[kr./Euro]</f>
+        <v>10.32171581769437</v>
+      </c>
+      <c r="D3" cm="1">
+        <f t="array" ref="D3">D2/Table1[kr./Euro]</f>
+        <v>10.32171581769437</v>
+      </c>
+      <c r="E3" cm="1">
+        <f t="array" ref="E3">E2/Table1[kr./Euro]</f>
+        <v>10.32171581769437</v>
+      </c>
+      <c r="F3" cm="1">
+        <f t="array" ref="F3">F2/Table1[kr./Euro]</f>
         <v>12.466487935656836</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>13</v>
       </c>
@@ -599,21 +770,122 @@
       </c>
       <c r="C4" cm="1">
         <f t="array" ref="C4">C3*Table3[Column1]</f>
+        <v>37.158176943699736</v>
+      </c>
+      <c r="D4" cm="1">
+        <f t="array" ref="D4">D3*Table3[Column1]</f>
+        <v>37.158176943699736</v>
+      </c>
+      <c r="E4" cm="1">
+        <f t="array" ref="E4">E3*Table3[Column1]</f>
+        <v>37.158176943699736</v>
+      </c>
+      <c r="F4" cm="1">
+        <f t="array" ref="F4">F3*Table3[Column1]</f>
         <v>44.879356568364614</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <tableParts count="1">
+    <tablePart r:id="rId2"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2DD5308E-2F08-462B-8525-5B5F16C7AE66}">
+  <dimension ref="A1:F6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E6" sqref="E6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="10.54296875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B2">
+        <v>7.46</v>
+      </c>
+      <c r="D2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E2">
+        <v>3.6</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>16</v>
+      </c>
+      <c r="B5" t="s">
+        <v>19</v>
+      </c>
+      <c r="C5" t="s">
+        <v>18</v>
+      </c>
+      <c r="D5" t="s">
+        <v>17</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>5</v>
+      </c>
+      <c r="B6">
+        <v>77</v>
+      </c>
+      <c r="C6">
+        <v>77</v>
+      </c>
+      <c r="D6">
+        <v>77</v>
+      </c>
+      <c r="E6" s="3">
+        <v>77</v>
+      </c>
+      <c r="F6" s="3">
+        <v>93</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="3">
+    <tablePart r:id="rId1"/>
     <tablePart r:id="rId2"/>
     <tablePart r:id="rId3"/>
-    <tablePart r:id="rId4"/>
   </tableParts>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0AC95DC8-DA49-4D29-8AB2-7E8DE05EEF12}">
   <dimension ref="A1:B3"/>
   <sheetViews>

</xml_diff>

<commit_message>
fix 2018 district heating price bug
</commit_message>
<xml_diff>
--- a/spine_projects/01_input_data/01_input_raw/energy_prices/district_heating_price_cap.xlsx
+++ b/spine_projects/01_input_data/01_input_raw/energy_prices/district_heating_price_cap.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27531"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27628"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jfg.eco\Documents\GitHub\Nord_H2ub\spine_projects\01_input_data\01_input_raw\energy_prices\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F00FFD3-894A-456A-96BF-9C096690F073}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{94DA13C8-180D-4980-BB9F-AA3F8C9D2A2E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{BDF52CB5-8AF7-4070-9BAF-21BBD77363FF}"/>
+    <workbookView xWindow="-5070" yWindow="-21720" windowWidth="38640" windowHeight="21120" xr2:uid="{BDF52CB5-8AF7-4070-9BAF-21BBD77363FF}"/>
   </bookViews>
   <sheets>
     <sheet name="Price_Cap_Calculation" sheetId="1" r:id="rId1"/>
@@ -60,7 +60,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="21">
   <si>
     <t>Law</t>
   </si>
@@ -120,6 +120,9 @@
   </si>
   <si>
     <t>2019</t>
+  </si>
+  <si>
+    <t>2018</t>
   </si>
 </sst>
 </file>
@@ -203,14 +206,34 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="4">
+  <dxfs count="6">
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="4" tint="0.79998168889431442"/>
+          <bgColor theme="4" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </top>
+        <bottom style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
     </dxf>
     <dxf>
       <font>
@@ -291,6 +314,9 @@
         </right>
       </border>
     </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -305,14 +331,17 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{8F68E1AD-1E8B-4ACE-A9DE-2514707D9B42}" name="Table4" displayName="Table4" ref="A1:F4" totalsRowShown="0">
-  <autoFilter ref="A1:F4" xr:uid="{8F68E1AD-1E8B-4ACE-A9DE-2514707D9B42}"/>
-  <tableColumns count="6">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{8F68E1AD-1E8B-4ACE-A9DE-2514707D9B42}" name="Table4" displayName="Table4" ref="A1:G4" totalsRowShown="0">
+  <autoFilter ref="A1:G4" xr:uid="{8F68E1AD-1E8B-4ACE-A9DE-2514707D9B42}"/>
+  <tableColumns count="7">
     <tableColumn id="1" xr3:uid="{A6FEAB50-FA63-446B-B963-FFE2083525E3}" name="Price cap"/>
+    <tableColumn id="8" xr3:uid="{F08150EC-6285-44C7-B582-FF0BA3697B79}" name="2018" dataDxfId="0">
+      <calculatedColumnFormula array="1">Table2[2018]</calculatedColumnFormula>
+    </tableColumn>
     <tableColumn id="2" xr3:uid="{E77E28C3-6031-4C08-B54D-35A5A0CCC2F3}" name="2019"/>
     <tableColumn id="3" xr3:uid="{9BF1D066-C7E0-4A13-8E0A-07795D412DD6}" name="2020"/>
-    <tableColumn id="4" xr3:uid="{94EEE701-C19A-4405-B469-9A9B9CFF43D5}" name="2021" dataDxfId="0">
-      <calculatedColumnFormula array="1">Table2[2019]</calculatedColumnFormula>
+    <tableColumn id="4" xr3:uid="{94EEE701-C19A-4405-B469-9A9B9CFF43D5}" name="2021" dataDxfId="5">
+      <calculatedColumnFormula array="1">Table2[2018]</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="5" xr3:uid="{8EC6DBC7-5CD1-4CC1-B48E-052446EA7F03}" name="2022"/>
     <tableColumn id="6" xr3:uid="{CE5F0BFC-0E32-4299-85B7-B0940B445FB9}" name="2023"/>
@@ -344,15 +373,16 @@
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{7BF6279C-0A47-4882-8A47-FBB883A7F586}" name="Table2" displayName="Table2" ref="A5:F6" totalsRowShown="0" tableBorderDxfId="3">
-  <autoFilter ref="A5:F6" xr:uid="{7BF6279C-0A47-4882-8A47-FBB883A7F586}"/>
-  <tableColumns count="6">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{7BF6279C-0A47-4882-8A47-FBB883A7F586}" name="Table2" displayName="Table2" ref="A5:G6" totalsRowShown="0" tableBorderDxfId="4">
+  <autoFilter ref="A5:G6" xr:uid="{7BF6279C-0A47-4882-8A47-FBB883A7F586}"/>
+  <tableColumns count="7">
     <tableColumn id="1" xr3:uid="{D3E85E44-117A-4A3D-B167-80884115B936}" name="Price cap"/>
-    <tableColumn id="2" xr3:uid="{9FB8A1A3-5B94-42D9-8374-F609ECDC4806}" name="2019"/>
-    <tableColumn id="3" xr3:uid="{BC877BDF-034D-4BAE-8945-44CE9F9FA3BF}" name="2020"/>
-    <tableColumn id="4" xr3:uid="{C3208B9F-5220-4737-97F7-04B4B458599B}" name="2021"/>
-    <tableColumn id="5" xr3:uid="{717424EF-4D50-42EC-ABE0-707DA0FB5BFE}" name="2022" dataDxfId="2"/>
-    <tableColumn id="6" xr3:uid="{7B8608B1-3E6A-44D6-B820-4DE5304A1F9D}" name="2023" dataDxfId="1"/>
+    <tableColumn id="2" xr3:uid="{9FB8A1A3-5B94-42D9-8374-F609ECDC4806}" name="2018"/>
+    <tableColumn id="3" xr3:uid="{BC877BDF-034D-4BAE-8945-44CE9F9FA3BF}" name="2019"/>
+    <tableColumn id="4" xr3:uid="{C3208B9F-5220-4737-97F7-04B4B458599B}" name="2020"/>
+    <tableColumn id="5" xr3:uid="{717424EF-4D50-42EC-ABE0-707DA0FB5BFE}" name="2021" dataDxfId="3"/>
+    <tableColumn id="6" xr3:uid="{7B8608B1-3E6A-44D6-B820-4DE5304A1F9D}" name="2022" dataDxfId="2"/>
+    <tableColumn id="7" xr3:uid="{B8C7C939-753F-4966-977C-1E33CD2C3DDD}" name="2023" dataDxfId="1"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -675,67 +705,74 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{38179E1F-D8DC-462A-A2B6-DE363F6626F8}">
-  <dimension ref="A1:F4"/>
+  <dimension ref="A1:G4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I11" sqref="I11"/>
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="10.453125" customWidth="1"/>
-    <col min="7" max="7" width="15" customWidth="1"/>
-    <col min="8" max="8" width="9.453125" customWidth="1"/>
-    <col min="10" max="10" width="12.453125" customWidth="1"/>
-    <col min="11" max="11" width="10.453125" customWidth="1"/>
+    <col min="1" max="2" width="10.453125" customWidth="1"/>
+    <col min="8" max="8" width="15" customWidth="1"/>
+    <col min="9" max="9" width="9.453125" customWidth="1"/>
+    <col min="11" max="11" width="12.453125" customWidth="1"/>
+    <col min="12" max="12" width="10.453125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>16</v>
       </c>
       <c r="B1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C1" t="s">
         <v>19</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>18</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>17</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="G1" s="2" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>5</v>
       </c>
       <c r="B2" cm="1">
-        <f t="array" ref="B2">Table2[2019]</f>
+        <f t="array" ref="B2">Table2[2018]</f>
         <v>77</v>
       </c>
       <c r="C2" cm="1">
-        <f t="array" ref="C2">Table2[2020]</f>
+        <f t="array" ref="C2">Table2[2019]</f>
         <v>77</v>
       </c>
       <c r="D2" cm="1">
-        <f t="array" ref="D2">Table2[2021]</f>
+        <f t="array" ref="D2">Table2[2020]</f>
         <v>77</v>
       </c>
       <c r="E2" cm="1">
-        <f t="array" ref="E2">Table2[2022]</f>
+        <f t="array" ref="E2">Table2[2021]</f>
         <v>77</v>
       </c>
       <c r="F2" cm="1">
-        <f t="array" ref="F2">Table2[2023]</f>
+        <f t="array" ref="F2">Table2[2022]</f>
+        <v>77</v>
+      </c>
+      <c r="G2" cm="1">
+        <f t="array" ref="G2">Table2[2023]</f>
         <v>93</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>9</v>
       </c>
@@ -757,10 +794,14 @@
       </c>
       <c r="F3" cm="1">
         <f t="array" ref="F3">F2/Table1[kr./Euro]</f>
+        <v>10.32171581769437</v>
+      </c>
+      <c r="G3" cm="1">
+        <f t="array" ref="G3">G2/Table1[kr./Euro]</f>
         <v>12.466487935656836</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>13</v>
       </c>
@@ -782,6 +823,10 @@
       </c>
       <c r="F4" cm="1">
         <f t="array" ref="F4">F3*Table3[Column1]</f>
+        <v>37.158176943699736</v>
+      </c>
+      <c r="G4" cm="1">
+        <f t="array" ref="G4">G3*Table3[Column1]</f>
         <v>44.879356568364614</v>
       </c>
     </row>
@@ -796,10 +841,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2DD5308E-2F08-462B-8525-5B5F16C7AE66}">
-  <dimension ref="A1:F6"/>
+  <dimension ref="A1:G6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -807,7 +852,7 @@
     <col min="1" max="1" width="10.54296875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>6</v>
       </c>
@@ -821,7 +866,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>8</v>
       </c>
@@ -835,27 +880,30 @@
         <v>3.6</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>16</v>
       </c>
       <c r="B5" t="s">
+        <v>20</v>
+      </c>
+      <c r="C5" t="s">
         <v>19</v>
       </c>
-      <c r="C5" t="s">
+      <c r="D5" t="s">
         <v>18</v>
       </c>
-      <c r="D5" t="s">
+      <c r="E5" t="s">
         <v>17</v>
       </c>
-      <c r="E5" s="1" t="s">
+      <c r="F5" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="F5" s="1" t="s">
+      <c r="G5" s="1" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>5</v>
       </c>
@@ -868,10 +916,13 @@
       <c r="D6">
         <v>77</v>
       </c>
-      <c r="E6" s="3">
+      <c r="E6">
         <v>77</v>
       </c>
       <c r="F6" s="3">
+        <v>77</v>
+      </c>
+      <c r="G6" s="3">
         <v>93</v>
       </c>
     </row>

</xml_diff>